<commit_message>
Menu Personnages Alpha 0.2
</commit_message>
<xml_diff>
--- a/Outiles/StatsPersonnages.xlsx
+++ b/Outiles/StatsPersonnages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E73A2108-55F4-4011-B7D2-1AFAB8B489F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B95EB-A79C-4D3E-836E-AC5BD1703D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Personages</t>
   </si>
@@ -122,13 +122,43 @@
   </si>
   <si>
     <t>Up_Personnage_8</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>name4</t>
+  </si>
+  <si>
+    <t>name5</t>
+  </si>
+  <si>
+    <t>name6</t>
+  </si>
+  <si>
+    <t>name7</t>
+  </si>
+  <si>
+    <t>name8</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +169,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -595,18 +631,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F46BB-8D66-4AFF-A145-FBCAA6808CDD}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -637,8 +673,14 @@
       <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -669,8 +711,14 @@
       <c r="J2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
@@ -701,8 +749,14 @@
       <c r="J3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -733,8 +787,14 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -765,8 +825,14 @@
       <c r="J5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -797,8 +863,14 @@
       <c r="J6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -829,8 +901,14 @@
       <c r="J7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -861,8 +939,14 @@
       <c r="J8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="1">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -893,8 +977,14 @@
       <c r="J9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -925,8 +1015,14 @@
       <c r="J10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -957,8 +1053,14 @@
       <c r="J11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -989,8 +1091,14 @@
       <c r="J12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -1021,8 +1129,14 @@
       <c r="J13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1053,8 +1167,14 @@
       <c r="J14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -1085,8 +1205,14 @@
       <c r="J15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1117,8 +1243,14 @@
       <c r="J16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -1149,8 +1281,15 @@
       <c r="J17" s="3">
         <v>0</v>
       </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>9999</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stat Caracters Alpla 0.22
</commit_message>
<xml_diff>
--- a/Outiles/StatsPersonnages.xlsx
+++ b/Outiles/StatsPersonnages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Documents\Code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B95EB-A79C-4D3E-836E-AC5BD1703D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0845FF1E-FC8B-411A-B2AF-DA0435D37409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
   </bookViews>
   <sheets>
     <sheet name="StatsPersonnages" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Personages</t>
   </si>
@@ -127,31 +127,46 @@
     <t>name</t>
   </si>
   <si>
-    <t>name1</t>
-  </si>
-  <si>
-    <t>name2</t>
-  </si>
-  <si>
-    <t>name3</t>
-  </si>
-  <si>
-    <t>name4</t>
-  </si>
-  <si>
-    <t>name5</t>
-  </si>
-  <si>
-    <t>name6</t>
-  </si>
-  <si>
-    <t>name7</t>
-  </si>
-  <si>
-    <t>name8</t>
-  </si>
-  <si>
     <t>price</t>
+  </si>
+  <si>
+    <t>Cyrdin</t>
+  </si>
+  <si>
+    <t>Galdir</t>
+  </si>
+  <si>
+    <t>Shoginawa</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>Nato</t>
+  </si>
+  <si>
+    <t>Djo</t>
+  </si>
+  <si>
+    <t>Nicox</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.3</t>
   </si>
 </sst>
 </file>
@@ -633,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F46BB-8D66-4AFF-A145-FBCAA6808CDD}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +692,7 @@
         <v>29</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -691,10 +706,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <v>300</v>
@@ -712,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
@@ -723,7 +738,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>13</v>
@@ -761,25 +776,25 @@
         <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F4" s="1">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -788,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="L4" s="1">
         <v>1000</v>
@@ -802,22 +817,22 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="I5" s="3">
         <v>0</v>
@@ -837,22 +852,22 @@
         <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="1">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="G6" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1">
         <v>8</v>
@@ -864,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L6" s="1">
         <v>2500</v>
@@ -883,14 +898,14 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>2</v>
+      <c r="E7" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F7" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>14</v>
@@ -913,26 +928,26 @@
         <v>19</v>
       </c>
       <c r="B8" s="1">
+        <v>250</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
         <v>100</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="G8" s="1">
+        <v>7</v>
+      </c>
+      <c r="H8" s="1">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>300</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>8</v>
-      </c>
       <c r="I8" s="1">
         <v>1</v>
       </c>
@@ -940,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L8" s="1">
         <v>7000</v>
@@ -951,7 +966,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="3">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
@@ -960,16 +975,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -989,7 +1004,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
@@ -998,25 +1013,25 @@
         <v>5</v>
       </c>
       <c r="E10" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1">
         <v>5</v>
       </c>
       <c r="H10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L10" s="1">
         <v>25000</v>
@@ -1027,7 +1042,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
@@ -1065,13 +1080,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="1">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
@@ -1092,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L12" s="1">
         <v>15000</v>
@@ -1103,7 +1118,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
@@ -1112,16 +1127,16 @@
         <v>0</v>
       </c>
       <c r="E13" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3">
         <v>10</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
@@ -1141,7 +1156,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -1153,22 +1168,22 @@
         <v>10</v>
       </c>
       <c r="F14" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G14" s="1">
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" s="1">
         <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L14" s="1">
         <v>50000</v>
@@ -1188,16 +1203,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>14</v>
+      <c r="H15" s="4">
+        <v>0</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
@@ -1217,16 +1232,16 @@
         <v>27</v>
       </c>
       <c r="B16" s="1">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1">
         <v>300</v>
@@ -1244,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L16" s="1">
         <v>100000</v>
@@ -1255,7 +1270,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="3">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
@@ -1264,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3">
         <v>10</v>
@@ -1273,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="I17" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Menu + Stats Caracters Aplha 0.23
</commit_message>
<xml_diff>
--- a/Outiles/StatsPersonnages.xlsx
+++ b/Outiles/StatsPersonnages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Documents\Code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0845FF1E-FC8B-411A-B2AF-DA0435D37409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF9297-06C2-4D07-AA6C-5673D22CB0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
+    <workbookView xWindow="53745" yWindow="5145" windowWidth="38700" windowHeight="15435" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
   </bookViews>
   <sheets>
     <sheet name="StatsPersonnages" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Personages</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Djo</t>
   </si>
   <si>
-    <t>Nicox</t>
-  </si>
-  <si>
     <t>0.2</t>
   </si>
   <si>
@@ -167,6 +164,27 @@
   </si>
   <si>
     <t>1.3</t>
+  </si>
+  <si>
+    <t>Kral</t>
+  </si>
+  <si>
+    <t>rechargeTime</t>
+  </si>
+  <si>
+    <t>weaponSpeed</t>
+  </si>
+  <si>
+    <t>weaponName</t>
+  </si>
+  <si>
+    <t>WeaponPrice</t>
+  </si>
+  <si>
+    <t>Shuriken</t>
+  </si>
+  <si>
+    <t>0.4</t>
   </si>
 </sst>
 </file>
@@ -297,7 +315,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,6 +345,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,18 +673,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F46BB-8D66-4AFF-A145-FBCAA6808CDD}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="20.7109375" customWidth="1"/>
+    <col min="1" max="20" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -680,22 +707,35 @@
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -717,23 +757,36 @@
       <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <v>8</v>
       </c>
-      <c r="I2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="12"/>
+    </row>
+    <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
@@ -755,23 +808,36 @@
       <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>500</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="13"/>
+    </row>
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -779,7 +845,7 @@
         <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
@@ -793,23 +859,36 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>6</v>
       </c>
-      <c r="I4" s="1">
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="O4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="12"/>
+    </row>
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -817,37 +896,50 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>700</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="13"/>
+    </row>
+    <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -869,23 +961,36 @@
       <c r="G6" s="1">
         <v>10</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="1">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>8</v>
       </c>
-      <c r="I6" s="1">
+      <c r="M6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1">
+      <c r="N6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="1">
+      <c r="P6" s="1">
         <v>2500</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="12"/>
+    </row>
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -899,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3">
         <v>50</v>
@@ -907,23 +1012,36 @@
       <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>800</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -931,7 +1049,7 @@
         <v>250</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1">
         <v>10</v>
@@ -945,23 +1063,36 @@
       <c r="G8" s="1">
         <v>7</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1">
+        <v>10</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>5</v>
       </c>
-      <c r="I8" s="1">
+      <c r="M8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1">
+      <c r="N8" s="1">
         <v>1</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="1">
+      <c r="P8" s="1">
         <v>7000</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="12"/>
+    </row>
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -983,8 +1114,8 @@
       <c r="G9" s="3">
         <v>0</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>39</v>
+      <c r="H9" s="4">
+        <v>0</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -993,13 +1124,26 @@
         <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1021,23 +1165,36 @@
       <c r="G10" s="1">
         <v>5</v>
       </c>
-      <c r="H10" s="1">
-        <v>10</v>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I10" s="1">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>10</v>
+      </c>
+      <c r="M10" s="1">
         <v>2</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="N10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="1">
+      <c r="P10" s="1">
         <v>25000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -1059,23 +1216,36 @@
       <c r="G11" s="3">
         <v>0</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>600</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1097,23 +1267,36 @@
       <c r="G12" s="1">
         <v>5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>8</v>
       </c>
-      <c r="I12" s="1">
+      <c r="M12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1">
+      <c r="N12" s="1">
         <v>1</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="1">
+      <c r="P12" s="1">
         <v>15000</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="12"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -1135,8 +1318,8 @@
       <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>39</v>
+      <c r="H13" s="4">
+        <v>0</v>
       </c>
       <c r="I13" s="3">
         <v>0</v>
@@ -1145,13 +1328,26 @@
         <v>0</v>
       </c>
       <c r="K13" s="3">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>2500</v>
+      </c>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1173,23 +1369,36 @@
       <c r="G14" s="1">
         <v>5</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="1">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
         <v>12</v>
       </c>
-      <c r="I14" s="1">
+      <c r="M14" s="1">
         <v>2</v>
       </c>
-      <c r="J14" s="1">
+      <c r="N14" s="1">
         <v>1</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="1">
+      <c r="P14" s="1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="12"/>
+    </row>
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -1221,13 +1430,26 @@
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
+        <v>2000</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1249,23 +1471,36 @@
       <c r="G16" s="1">
         <v>5</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="1">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
         <v>8</v>
       </c>
-      <c r="I16" s="1">
+      <c r="M16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1">
+      <c r="N16" s="1">
         <v>1</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="1">
+      <c r="P16" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="12"/>
+    </row>
+    <row r="17" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
@@ -1287,8 +1522,8 @@
       <c r="G17" s="3">
         <v>0</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>39</v>
+      <c r="H17" s="4">
+        <v>0</v>
       </c>
       <c r="I17" s="3">
         <v>0</v>
@@ -1297,11 +1532,24 @@
         <v>0</v>
       </c>
       <c r="K17" s="3">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3">
+        <v>5000</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
         <v>9999</v>
       </c>
+      <c r="Q17" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
ajout des différente armes
</commit_message>
<xml_diff>
--- a/Outiles/StatsPersonnages.xlsx
+++ b/Outiles/StatsPersonnages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Documents\Code\GitHub\Jeu-Dzarian-Miniquoinquoin\Outiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF9297-06C2-4D07-AA6C-5673D22CB0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDABA98A-E1E0-47C8-93A5-E3FB6060E2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53745" yWindow="5145" windowWidth="38700" windowHeight="15435" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{26D64052-F692-4786-847A-089B52D9574B}"/>
   </bookViews>
   <sheets>
     <sheet name="StatsPersonnages" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Personages</t>
   </si>
@@ -185,6 +185,27 @@
   </si>
   <si>
     <t>0.4</t>
+  </si>
+  <si>
+    <t>Dague</t>
+  </si>
+  <si>
+    <t>BouleElectrique</t>
+  </si>
+  <si>
+    <t>Epee</t>
+  </si>
+  <si>
+    <t>Lance</t>
+  </si>
+  <si>
+    <t>Hache</t>
+  </si>
+  <si>
+    <t>Flechette</t>
+  </si>
+  <si>
+    <t>BouleDeFeu</t>
   </si>
 </sst>
 </file>
@@ -676,7 +697,10 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +788,7 @@
         <v>10</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
@@ -866,7 +890,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -956,7 +980,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="1">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="G6" s="1">
         <v>10</v>
@@ -968,7 +992,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -1070,7 +1094,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -1160,7 +1184,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G10" s="1">
         <v>5</v>
@@ -1169,10 +1193,10 @@
         <v>40</v>
       </c>
       <c r="I10" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -1211,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -1274,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K12" s="1">
         <v>0</v>
@@ -1376,7 +1400,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="K14" s="1">
         <v>0</v>
@@ -1553,6 +1577,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;A</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>